<commit_message>
Concept 2 versie, mist alleen conclusie MT, final conclusion, samenvatting en voorwoord
</commit_message>
<xml_diff>
--- a/Other/Uitnodigingen AfstudeerBorrel.xlsx
+++ b/Other/Uitnodigingen AfstudeerBorrel.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d4f24f3f093ab16/Studie/Thesis/Other/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ingma\OneDrive\Studie\Thesis\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="97C32B1B612C4FF45CF30E7DD16AE2B5ABE31D7D" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{228099A4-C76A-4CA4-8588-8160B9ECCAF8}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="97C32B1B612C4FF45CF30E7DD16AE2B5ABE31D7D" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{B1DDA68B-8D37-40BD-B08C-127E7DB5C0FC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{7D570AA1-68F6-495A-A5B0-8503DD956D61}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{7D570AA1-68F6-495A-A5B0-8503DD956D61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="232">
   <si>
     <t>Assendelft</t>
   </si>
@@ -703,6 +708,24 @@
   </si>
   <si>
     <t>Guerrera Galan</t>
+  </si>
+  <si>
+    <t>Wilma</t>
+  </si>
+  <si>
+    <t>Hiemstra</t>
+  </si>
+  <si>
+    <t>Knipscheer</t>
+  </si>
+  <si>
+    <t>Peer</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>Nanhekan</t>
   </si>
 </sst>
 </file>
@@ -742,7 +765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -760,7 +783,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -797,7 +820,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -884,7 +907,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>4</c:v>
@@ -952,7 +975,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="80433712"/>
@@ -1011,7 +1034,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2040374400"/>
@@ -1059,7 +1082,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1657,7 +1680,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5263348-6439-4EA1-83DE-16211CED91AF}" name="Table1" displayName="Table1" ref="A1:C1048576" totalsRowShown="0">
   <autoFilter ref="A1:C1048576" xr:uid="{E76780AD-23FF-417D-AAB9-DFC36D556B45}"/>
-  <sortState ref="A2:C125">
+  <sortState ref="A2:C130">
     <sortCondition ref="C1:C1048576"/>
   </sortState>
   <tableColumns count="3">
@@ -1670,7 +1693,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1966,10 +1989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AC7B75-1DE5-4D40-B752-8E8AAB6D235A}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2131,7 +2154,7 @@
       </c>
       <c r="G9">
         <f>COUNTIF(Table1[[#All],[Reden]],F9)</f>
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2189,7 +2212,7 @@
       </c>
       <c r="G13">
         <f>SUM(G2:G12)</f>
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2227,10 +2250,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>223</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>224</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
@@ -2238,10 +2261,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
@@ -2249,21 +2272,21 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="C19" t="s">
-        <v>221</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C20" t="s">
         <v>221</v>
@@ -2271,10 +2294,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B21" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C21" t="s">
         <v>221</v>
@@ -2282,10 +2305,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B22" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C22" t="s">
         <v>221</v>
@@ -2293,10 +2316,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C23" t="s">
         <v>221</v>
@@ -2304,21 +2327,21 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>143</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="C24" t="s">
-        <v>153</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>143</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>206</v>
       </c>
       <c r="C25" t="s">
         <v>153</v>
@@ -2326,10 +2349,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>205</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
         <v>153</v>
@@ -2337,10 +2360,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C27" t="s">
         <v>153</v>
@@ -2348,21 +2371,21 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C28" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>212</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>213</v>
       </c>
       <c r="C29" t="s">
         <v>148</v>
@@ -2370,10 +2393,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
         <v>148</v>
@@ -2381,10 +2404,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
         <v>148</v>
@@ -2392,10 +2415,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
         <v>148</v>
@@ -2403,10 +2426,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="C33" t="s">
         <v>148</v>
@@ -2414,10 +2437,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
         <v>148</v>
@@ -2425,10 +2448,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
         <v>148</v>
@@ -2436,10 +2459,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="C36" t="s">
         <v>148</v>
@@ -2447,10 +2470,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="B37" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C37" t="s">
         <v>148</v>
@@ -2458,21 +2481,21 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>179</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -2480,10 +2503,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -2491,10 +2514,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>196</v>
+        <v>11</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -2502,10 +2525,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>9</v>
+        <v>196</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -2513,10 +2536,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -2524,21 +2547,21 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>150</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>214</v>
+        <v>71</v>
       </c>
       <c r="B45" t="s">
-        <v>215</v>
+        <v>72</v>
       </c>
       <c r="C45" t="s">
         <v>150</v>
@@ -2546,10 +2569,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="B46" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="C46" t="s">
         <v>150</v>
@@ -2557,10 +2580,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="B47" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="C47" t="s">
         <v>150</v>
@@ -2568,10 +2591,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>219</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>220</v>
       </c>
       <c r="C48" t="s">
         <v>150</v>
@@ -2579,10 +2602,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C49" t="s">
         <v>150</v>
@@ -2590,10 +2613,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="C50" t="s">
         <v>150</v>
@@ -2601,10 +2624,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="C51" t="s">
         <v>150</v>
@@ -2612,10 +2635,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
         <v>150</v>
@@ -2623,10 +2646,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C53" t="s">
         <v>150</v>
@@ -2634,10 +2657,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>216</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>217</v>
+        <v>68</v>
       </c>
       <c r="C54" t="s">
         <v>150</v>
@@ -2645,10 +2668,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>216</v>
       </c>
       <c r="B55" t="s">
-        <v>88</v>
+        <v>217</v>
       </c>
       <c r="C55" t="s">
         <v>150</v>
@@ -2656,10 +2679,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="C56" t="s">
         <v>150</v>
@@ -2667,10 +2690,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="B57" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="C57" t="s">
         <v>150</v>
@@ -2678,13 +2701,13 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>223</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>224</v>
+        <v>91</v>
       </c>
       <c r="C58" t="s">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2755,10 +2778,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>116</v>
+        <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="C65" t="s">
         <v>152</v>
@@ -2766,10 +2789,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B66" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C66" t="s">
         <v>152</v>
@@ -2777,10 +2800,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="B67" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="C67" t="s">
         <v>152</v>
@@ -2788,10 +2811,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="C68" t="s">
         <v>152</v>
@@ -2799,10 +2822,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>146</v>
+        <v>14</v>
       </c>
       <c r="B69" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="C69" t="s">
         <v>152</v>
@@ -2810,10 +2833,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="B70" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="C70" t="s">
         <v>152</v>
@@ -2821,10 +2844,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="B71" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="C71" t="s">
         <v>152</v>
@@ -2832,10 +2855,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="B72" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="C72" t="s">
         <v>152</v>
@@ -2843,10 +2866,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>194</v>
+        <v>112</v>
       </c>
       <c r="B73" t="s">
-        <v>195</v>
+        <v>113</v>
       </c>
       <c r="C73" t="s">
         <v>152</v>
@@ -2854,10 +2877,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>114</v>
+        <v>194</v>
       </c>
       <c r="B74" t="s">
-        <v>115</v>
+        <v>195</v>
       </c>
       <c r="C74" t="s">
         <v>152</v>
@@ -2865,10 +2888,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="B75" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="C75" t="s">
         <v>152</v>
@@ -2876,10 +2899,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B76" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="C76" t="s">
         <v>152</v>
@@ -2887,10 +2910,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C77" t="s">
         <v>152</v>
@@ -2898,10 +2921,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="C78" t="s">
         <v>152</v>
@@ -2912,7 +2935,7 @@
         <v>118</v>
       </c>
       <c r="B79" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C79" t="s">
         <v>152</v>
@@ -2920,10 +2943,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B80" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C80" t="s">
         <v>152</v>
@@ -2931,10 +2954,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B81" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C81" t="s">
         <v>152</v>
@@ -2942,10 +2965,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>197</v>
+        <v>132</v>
       </c>
       <c r="B82" t="s">
-        <v>198</v>
+        <v>133</v>
       </c>
       <c r="C82" t="s">
         <v>152</v>
@@ -2953,10 +2976,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>123</v>
+        <v>197</v>
       </c>
       <c r="B83" t="s">
-        <v>124</v>
+        <v>198</v>
       </c>
       <c r="C83" t="s">
         <v>152</v>
@@ -2964,10 +2987,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>43</v>
+        <v>123</v>
       </c>
       <c r="B84" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C84" t="s">
         <v>152</v>
@@ -2975,10 +2998,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B85" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="C85" t="s">
         <v>152</v>
@@ -2986,10 +3009,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="B86" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="C86" t="s">
         <v>152</v>
@@ -2997,10 +3020,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B87" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="C87" t="s">
         <v>152</v>
@@ -3011,7 +3034,7 @@
         <v>45</v>
       </c>
       <c r="B88" t="s">
-        <v>182</v>
+        <v>139</v>
       </c>
       <c r="C88" t="s">
         <v>152</v>
@@ -3019,10 +3042,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>199</v>
+        <v>45</v>
       </c>
       <c r="B89" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="C89" t="s">
         <v>152</v>
@@ -3030,10 +3053,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>126</v>
+        <v>199</v>
       </c>
       <c r="B90" t="s">
-        <v>127</v>
+        <v>200</v>
       </c>
       <c r="C90" t="s">
         <v>152</v>
@@ -3041,10 +3064,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B91" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C91" t="s">
         <v>152</v>
@@ -3052,10 +3075,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B92" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C92" t="s">
         <v>152</v>
@@ -3063,10 +3086,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="B93" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
       <c r="C93" t="s">
         <v>152</v>
@@ -3074,10 +3097,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="B94" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="C94" t="s">
         <v>152</v>
@@ -3085,10 +3108,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="B95" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C95" t="s">
         <v>152</v>
@@ -3096,10 +3119,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
       <c r="B96" t="s">
-        <v>225</v>
+        <v>93</v>
       </c>
       <c r="C96" t="s">
         <v>152</v>
@@ -3107,10 +3130,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="B97" t="s">
-        <v>154</v>
+        <v>225</v>
       </c>
       <c r="C97" t="s">
         <v>152</v>
@@ -3382,45 +3405,97 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>14</v>
+        <v>226</v>
       </c>
       <c r="B122" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C122" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>83</v>
+        <v>3</v>
       </c>
       <c r="B123" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="C123" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>209</v>
-      </c>
-      <c r="B124" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="C124" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>230</v>
+      </c>
+      <c r="B125" t="s">
+        <v>231</v>
+      </c>
+      <c r="C125" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>190</v>
+      </c>
+      <c r="B126" t="s">
+        <v>215</v>
+      </c>
+      <c r="C126" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>14</v>
+      </c>
+      <c r="B127" t="s">
+        <v>222</v>
+      </c>
+      <c r="C127" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>83</v>
+      </c>
+      <c r="B128" t="s">
+        <v>211</v>
+      </c>
+      <c r="C128" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>209</v>
+      </c>
+      <c r="B129" t="s">
+        <v>210</v>
+      </c>
+      <c r="C129" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>207</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B130" t="s">
         <v>208</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C130" t="s">
         <v>149</v>
       </c>
     </row>

</xml_diff>